<commit_message>
Helper files from data requests
</commit_message>
<xml_diff>
--- a/PublicRecords/EPD-2025-4432_FlockUserAccount[2509-01]/Users_October_2_2025.table.xlsx
+++ b/PublicRecords/EPD-2025-4432_FlockUserAccount[2509-01]/Users_October_2_2025.table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoecs-my.sharepoint.com/personal/sethm_uoecs_org/Documents/Personal/EOE/repos/eugene-oregon/PublicRecords/EPD-2025-4432_FlockUserAccount[2509-01]/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{656BCB94-0386-4BEF-A45A-6B475A83B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46B50BA2-42B8-49AC-AD75-1D9A5FDFE405}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{656BCB94-0386-4BEF-A45A-6B475A83B9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E615CBF-03C2-47C5-B7CA-2550F1F8F6D3}"/>
   <bookViews>
     <workbookView xWindow="-57697" yWindow="-8160" windowWidth="28995" windowHeight="15675" xr2:uid="{2C88DD19-4D09-4752-BA9D-94500F7BCEAA}"/>
   </bookViews>
@@ -2197,7 +2197,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2991898A-FBF8-4F99-9345-AC05A1818212}" name="Table1" displayName="Table1" ref="A1:K195" totalsRowShown="0">
   <autoFilter ref="A1:K195" xr:uid="{2991898A-FBF8-4F99-9345-AC05A1818212}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K195">
-    <sortCondition descending="1" ref="K1:K195"/>
+    <sortCondition ref="I1:I195"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{882E49CD-DC4C-4FF3-A1C4-9B8D43F399A7}" name="First Name"/>
@@ -2536,7 +2536,8 @@
   <dimension ref="A1:K195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7018,30 +7019,42 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
       <c r="B157" t="s">
-        <v>66</v>
+        <v>220</v>
       </c>
       <c r="C157" t="s">
-        <v>67</v>
+        <v>221</v>
+      </c>
+      <c r="F157" t="s">
+        <v>21</v>
       </c>
       <c r="G157" t="s">
         <v>22</v>
       </c>
+      <c r="H157" t="s">
+        <v>16</v>
+      </c>
+      <c r="I157" t="s">
+        <v>17</v>
+      </c>
+      <c r="J157" t="s">
+        <v>17</v>
+      </c>
       <c r="K157" s="1">
-        <v>45860</v>
+        <v>45857</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>219</v>
+        <v>38</v>
       </c>
       <c r="B158" t="s">
-        <v>220</v>
+        <v>39</v>
       </c>
       <c r="C158" t="s">
-        <v>221</v>
+        <v>40</v>
       </c>
       <c r="F158" t="s">
         <v>21</v>
@@ -7059,27 +7072,27 @@
         <v>17</v>
       </c>
       <c r="K158" s="1">
-        <v>45857</v>
+        <v>45855</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>38</v>
+        <v>422</v>
       </c>
       <c r="B159" t="s">
-        <v>39</v>
+        <v>423</v>
       </c>
       <c r="C159" t="s">
-        <v>40</v>
+        <v>424</v>
       </c>
       <c r="F159" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="G159" t="s">
         <v>22</v>
       </c>
       <c r="H159" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I159" t="s">
         <v>17</v>
@@ -7093,22 +7106,22 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>422</v>
+        <v>246</v>
       </c>
       <c r="B160" t="s">
-        <v>423</v>
+        <v>247</v>
       </c>
       <c r="C160" t="s">
-        <v>424</v>
+        <v>248</v>
       </c>
       <c r="F160" t="s">
-        <v>77</v>
+        <v>21</v>
       </c>
       <c r="G160" t="s">
         <v>22</v>
       </c>
       <c r="H160" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I160" t="s">
         <v>17</v>
@@ -7117,21 +7130,21 @@
         <v>17</v>
       </c>
       <c r="K160" s="1">
-        <v>45855</v>
+        <v>45853</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>246</v>
+        <v>380</v>
       </c>
       <c r="B161" t="s">
-        <v>247</v>
+        <v>381</v>
       </c>
       <c r="C161" t="s">
-        <v>248</v>
+        <v>382</v>
       </c>
       <c r="F161" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G161" t="s">
         <v>22</v>
@@ -7146,21 +7159,21 @@
         <v>17</v>
       </c>
       <c r="K161" s="1">
-        <v>45853</v>
+        <v>45852</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>380</v>
+        <v>195</v>
       </c>
       <c r="B162" t="s">
-        <v>381</v>
+        <v>196</v>
       </c>
       <c r="C162" t="s">
-        <v>382</v>
+        <v>197</v>
       </c>
       <c r="F162" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G162" t="s">
         <v>22</v>
@@ -7175,18 +7188,18 @@
         <v>17</v>
       </c>
       <c r="K162" s="1">
-        <v>45852</v>
+        <v>45851</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="B163" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="C163" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="F163" t="s">
         <v>21</v>
@@ -7204,21 +7217,21 @@
         <v>17</v>
       </c>
       <c r="K163" s="1">
-        <v>45851</v>
+        <v>45845</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="B164" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="C164" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="F164" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G164" t="s">
         <v>22</v>
@@ -7233,18 +7246,18 @@
         <v>17</v>
       </c>
       <c r="K164" s="1">
-        <v>45845</v>
+        <v>45842</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>489</v>
       </c>
       <c r="B165" t="s">
-        <v>24</v>
+        <v>490</v>
       </c>
       <c r="C165" t="s">
-        <v>25</v>
+        <v>491</v>
       </c>
       <c r="F165" t="s">
         <v>26</v>
@@ -7262,18 +7275,18 @@
         <v>17</v>
       </c>
       <c r="K165" s="1">
-        <v>45842</v>
+        <v>45837</v>
       </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>489</v>
+        <v>408</v>
       </c>
       <c r="B166" t="s">
-        <v>490</v>
+        <v>409</v>
       </c>
       <c r="C166" t="s">
-        <v>491</v>
+        <v>410</v>
       </c>
       <c r="F166" t="s">
         <v>26</v>
@@ -7291,24 +7304,27 @@
         <v>17</v>
       </c>
       <c r="K166" s="1">
-        <v>45837</v>
+        <v>45836</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>408</v>
+        <v>11</v>
       </c>
       <c r="B167" t="s">
-        <v>409</v>
+        <v>12</v>
       </c>
       <c r="C167" t="s">
-        <v>410</v>
+        <v>13</v>
+      </c>
+      <c r="E167" t="s">
+        <v>14</v>
       </c>
       <c r="F167" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G167" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H167" t="s">
         <v>16</v>
@@ -7320,27 +7336,24 @@
         <v>17</v>
       </c>
       <c r="K167" s="1">
-        <v>45836</v>
+        <v>45832</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B168" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="C168" t="s">
-        <v>13</v>
-      </c>
-      <c r="E168" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="F168" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G168" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H168" t="s">
         <v>16</v>
@@ -7352,18 +7365,18 @@
         <v>17</v>
       </c>
       <c r="K168" s="1">
-        <v>45832</v>
+        <v>45830</v>
       </c>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="B169" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="C169" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="F169" t="s">
         <v>21</v>
@@ -7381,21 +7394,21 @@
         <v>17</v>
       </c>
       <c r="K169" s="1">
-        <v>45830</v>
+        <v>45824</v>
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>32</v>
+        <v>172</v>
       </c>
       <c r="B170" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
       <c r="C170" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="F170" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G170" t="s">
         <v>22</v>
@@ -7410,21 +7423,21 @@
         <v>17</v>
       </c>
       <c r="K170" s="1">
-        <v>45824</v>
+        <v>45823</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B171" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C171" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="F171" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G171" t="s">
         <v>22</v>
@@ -7439,18 +7452,18 @@
         <v>17</v>
       </c>
       <c r="K171" s="1">
-        <v>45823</v>
+        <v>45821</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>178</v>
+        <v>496</v>
       </c>
       <c r="B172" t="s">
-        <v>179</v>
+        <v>497</v>
       </c>
       <c r="C172" t="s">
-        <v>180</v>
+        <v>498</v>
       </c>
       <c r="F172" t="s">
         <v>21</v>
@@ -7473,16 +7486,16 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>496</v>
+        <v>50</v>
       </c>
       <c r="B173" t="s">
-        <v>497</v>
+        <v>51</v>
       </c>
       <c r="C173" t="s">
-        <v>498</v>
+        <v>52</v>
       </c>
       <c r="F173" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G173" t="s">
         <v>22</v>
@@ -7497,21 +7510,21 @@
         <v>17</v>
       </c>
       <c r="K173" s="1">
-        <v>45821</v>
+        <v>45820</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>50</v>
+        <v>271</v>
       </c>
       <c r="B174" t="s">
-        <v>51</v>
+        <v>272</v>
       </c>
       <c r="C174" t="s">
-        <v>52</v>
+        <v>273</v>
       </c>
       <c r="F174" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G174" t="s">
         <v>22</v>
@@ -7531,13 +7544,13 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>271</v>
+        <v>331</v>
       </c>
       <c r="B175" t="s">
-        <v>272</v>
+        <v>332</v>
       </c>
       <c r="C175" t="s">
-        <v>273</v>
+        <v>333</v>
       </c>
       <c r="F175" t="s">
         <v>21</v>
@@ -7560,13 +7573,13 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>331</v>
+        <v>505</v>
       </c>
       <c r="B176" t="s">
-        <v>332</v>
+        <v>506</v>
       </c>
       <c r="C176" t="s">
-        <v>333</v>
+        <v>507</v>
       </c>
       <c r="F176" t="s">
         <v>21</v>
@@ -7589,13 +7602,13 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>505</v>
+        <v>298</v>
       </c>
       <c r="B177" t="s">
-        <v>506</v>
+        <v>301</v>
       </c>
       <c r="C177" t="s">
-        <v>507</v>
+        <v>302</v>
       </c>
       <c r="F177" t="s">
         <v>21</v>
@@ -7613,21 +7626,33 @@
         <v>17</v>
       </c>
       <c r="K177" s="1">
-        <v>45820</v>
+        <v>45819</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>204</v>
+        <v>425</v>
       </c>
       <c r="B178" t="s">
-        <v>205</v>
+        <v>426</v>
       </c>
       <c r="C178" t="s">
-        <v>206</v>
+        <v>427</v>
+      </c>
+      <c r="F178" t="s">
+        <v>21</v>
       </c>
       <c r="G178" t="s">
         <v>22</v>
+      </c>
+      <c r="H178" t="s">
+        <v>16</v>
+      </c>
+      <c r="I178" t="s">
+        <v>17</v>
+      </c>
+      <c r="J178" t="s">
+        <v>17</v>
       </c>
       <c r="K178" s="1">
         <v>45819</v>
@@ -7635,13 +7660,13 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>298</v>
+        <v>56</v>
       </c>
       <c r="B179" t="s">
-        <v>301</v>
+        <v>57</v>
       </c>
       <c r="C179" t="s">
-        <v>302</v>
+        <v>58</v>
       </c>
       <c r="F179" t="s">
         <v>21</v>
@@ -7659,18 +7684,18 @@
         <v>17</v>
       </c>
       <c r="K179" s="1">
-        <v>45819</v>
+        <v>45818</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>425</v>
+        <v>78</v>
       </c>
       <c r="B180" t="s">
-        <v>426</v>
+        <v>79</v>
       </c>
       <c r="C180" t="s">
-        <v>427</v>
+        <v>80</v>
       </c>
       <c r="F180" t="s">
         <v>21</v>
@@ -7688,18 +7713,18 @@
         <v>17</v>
       </c>
       <c r="K180" s="1">
-        <v>45819</v>
+        <v>45818</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>56</v>
+        <v>439</v>
       </c>
       <c r="B181" t="s">
-        <v>57</v>
+        <v>442</v>
       </c>
       <c r="C181" t="s">
-        <v>58</v>
+        <v>443</v>
       </c>
       <c r="F181" t="s">
         <v>21</v>
@@ -7722,13 +7747,13 @@
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>78</v>
+        <v>477</v>
       </c>
       <c r="B182" t="s">
-        <v>79</v>
+        <v>478</v>
       </c>
       <c r="C182" t="s">
-        <v>80</v>
+        <v>479</v>
       </c>
       <c r="F182" t="s">
         <v>21</v>
@@ -7746,18 +7771,18 @@
         <v>17</v>
       </c>
       <c r="K182" s="1">
-        <v>45818</v>
+        <v>45815</v>
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>439</v>
+        <v>59</v>
       </c>
       <c r="B183" t="s">
-        <v>442</v>
+        <v>60</v>
       </c>
       <c r="C183" t="s">
-        <v>443</v>
+        <v>61</v>
       </c>
       <c r="F183" t="s">
         <v>21</v>
@@ -7775,38 +7800,50 @@
         <v>17</v>
       </c>
       <c r="K183" s="1">
-        <v>45818</v>
+        <v>45812</v>
       </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>508</v>
+        <v>383</v>
       </c>
       <c r="B184" t="s">
-        <v>509</v>
+        <v>384</v>
       </c>
       <c r="C184" t="s">
-        <v>510</v>
+        <v>385</v>
+      </c>
+      <c r="F184" t="s">
+        <v>21</v>
       </c>
       <c r="G184" t="s">
         <v>22</v>
       </c>
+      <c r="H184" t="s">
+        <v>16</v>
+      </c>
+      <c r="I184" t="s">
+        <v>17</v>
+      </c>
+      <c r="J184" t="s">
+        <v>17</v>
+      </c>
       <c r="K184" s="1">
-        <v>45816</v>
+        <v>45812</v>
       </c>
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>477</v>
+        <v>286</v>
       </c>
       <c r="B185" t="s">
-        <v>478</v>
+        <v>287</v>
       </c>
       <c r="C185" t="s">
-        <v>479</v>
+        <v>288</v>
       </c>
       <c r="F185" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G185" t="s">
         <v>22</v>
@@ -7821,21 +7858,21 @@
         <v>17</v>
       </c>
       <c r="K185" s="1">
-        <v>45815</v>
+        <v>45811</v>
       </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>59</v>
+        <v>261</v>
       </c>
       <c r="B186" t="s">
-        <v>60</v>
+        <v>262</v>
       </c>
       <c r="C186" t="s">
-        <v>61</v>
+        <v>263</v>
       </c>
       <c r="F186" t="s">
-        <v>21</v>
+        <v>264</v>
       </c>
       <c r="G186" t="s">
         <v>22</v>
@@ -7847,30 +7884,30 @@
         <v>17</v>
       </c>
       <c r="J186" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K186" s="1">
-        <v>45812</v>
+        <v>45807</v>
       </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>383</v>
+        <v>480</v>
       </c>
       <c r="B187" t="s">
-        <v>384</v>
+        <v>481</v>
       </c>
       <c r="C187" t="s">
-        <v>385</v>
+        <v>482</v>
       </c>
       <c r="F187" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="G187" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H187" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I187" t="s">
         <v>17</v>
@@ -7879,94 +7916,58 @@
         <v>17</v>
       </c>
       <c r="K187" s="1">
-        <v>45812</v>
+        <v>45807</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>286</v>
+        <v>65</v>
       </c>
       <c r="B188" t="s">
-        <v>287</v>
+        <v>66</v>
       </c>
       <c r="C188" t="s">
-        <v>288</v>
-      </c>
-      <c r="F188" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="G188" t="s">
         <v>22</v>
       </c>
-      <c r="H188" t="s">
-        <v>16</v>
-      </c>
-      <c r="I188" t="s">
-        <v>17</v>
-      </c>
-      <c r="J188" t="s">
-        <v>17</v>
-      </c>
       <c r="K188" s="1">
-        <v>45811</v>
+        <v>45860</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>261</v>
+        <v>204</v>
       </c>
       <c r="B189" t="s">
-        <v>262</v>
+        <v>205</v>
       </c>
       <c r="C189" t="s">
-        <v>263</v>
-      </c>
-      <c r="F189" t="s">
-        <v>264</v>
+        <v>206</v>
       </c>
       <c r="G189" t="s">
         <v>22</v>
       </c>
-      <c r="H189" t="s">
-        <v>16</v>
-      </c>
-      <c r="I189" t="s">
-        <v>17</v>
-      </c>
-      <c r="J189" t="s">
-        <v>16</v>
-      </c>
       <c r="K189" s="1">
-        <v>45807</v>
+        <v>45819</v>
       </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>480</v>
+        <v>508</v>
       </c>
       <c r="B190" t="s">
-        <v>481</v>
+        <v>509</v>
       </c>
       <c r="C190" t="s">
-        <v>482</v>
-      </c>
-      <c r="F190" t="s">
-        <v>77</v>
+        <v>510</v>
       </c>
       <c r="G190" t="s">
-        <v>15</v>
-      </c>
-      <c r="H190" t="s">
-        <v>17</v>
-      </c>
-      <c r="I190" t="s">
-        <v>17</v>
-      </c>
-      <c r="J190" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K190" s="1">
-        <v>45807</v>
+        <v>45816</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>